<commit_message>
Reports page redirection bug fixed.
</commit_message>
<xml_diff>
--- a/input_output.xlsx
+++ b/input_output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="242">
   <si>
     <t>asetickers</t>
   </si>
@@ -33,6 +33,714 @@
   </si>
   <si>
     <t>2022</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Non-current assets</t>
+  </si>
+  <si>
+    <t>Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>9,292,964</t>
+  </si>
+  <si>
+    <t>9,602,211</t>
+  </si>
+  <si>
+    <t>Intangible assets</t>
+  </si>
+  <si>
+    <t>11,308,218</t>
+  </si>
+  <si>
+    <t>Investment property</t>
+  </si>
+  <si>
+    <t>Investments in subsidiaries, joint ventures and associates</t>
+  </si>
+  <si>
+    <t>Financial assets at fair value through other comprehensive income</t>
+  </si>
+  <si>
+    <t>Financial assets at amortized cost</t>
+  </si>
+  <si>
+    <t>Non-current receivables due from related parties</t>
+  </si>
+  <si>
+    <t>Deferred tax assets</t>
+  </si>
+  <si>
+    <t>2,732,421</t>
+  </si>
+  <si>
+    <t>Trade and other non-current receivables</t>
+  </si>
+  <si>
+    <t>Other investments, including derivatives</t>
+  </si>
+  <si>
+    <t>Projects under implementation</t>
+  </si>
+  <si>
+    <t>Other non-current assets</t>
+  </si>
+  <si>
+    <t>Total non-current assets</t>
+  </si>
+  <si>
+    <t>23,333,603</t>
+  </si>
+  <si>
+    <t>23,642,850</t>
+  </si>
+  <si>
+    <t>Current assets</t>
+  </si>
+  <si>
+    <t>Current inventories</t>
+  </si>
+  <si>
+    <t>365,143</t>
+  </si>
+  <si>
+    <t>410,974</t>
+  </si>
+  <si>
+    <t>Trade and other current receivables</t>
+  </si>
+  <si>
+    <t>16,292,334</t>
+  </si>
+  <si>
+    <t>15,595,909</t>
+  </si>
+  <si>
+    <t>Financial assets at fair value through profit or loss</t>
+  </si>
+  <si>
+    <t>Current receivables due from related parties</t>
+  </si>
+  <si>
+    <t>104,231</t>
+  </si>
+  <si>
+    <t>1,082</t>
+  </si>
+  <si>
+    <t>Current loans and advances from employees</t>
+  </si>
+  <si>
+    <t>Cash on hand and at banks</t>
+  </si>
+  <si>
+    <t>164,479</t>
+  </si>
+  <si>
+    <t>190,609</t>
+  </si>
+  <si>
+    <t>Other current assets</t>
+  </si>
+  <si>
+    <t>Assets held for sale</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Total current assets</t>
+  </si>
+  <si>
+    <t>16,926,188</t>
+  </si>
+  <si>
+    <t>16,198,575</t>
+  </si>
+  <si>
+    <t>Total assets</t>
+  </si>
+  <si>
+    <t>40,259,791</t>
+  </si>
+  <si>
+    <t>39,841,425</t>
+  </si>
+  <si>
+    <t>Equity and liabilities</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Paid-up capital</t>
+  </si>
+  <si>
+    <t>15,000,000</t>
+  </si>
+  <si>
+    <t>Retained earnings</t>
+  </si>
+  <si>
+    <t>240,529</t>
+  </si>
+  <si>
+    <t>-8,229,717</t>
+  </si>
+  <si>
+    <t>Share premium</t>
+  </si>
+  <si>
+    <t>Issuance discount</t>
+  </si>
+  <si>
+    <t>Treasury shares</t>
+  </si>
+  <si>
+    <t>Other equity interest</t>
+  </si>
+  <si>
+    <t>Statutory reserve</t>
+  </si>
+  <si>
+    <t>257,406</t>
+  </si>
+  <si>
+    <t>Voluntary reserve</t>
+  </si>
+  <si>
+    <t>12,670</t>
+  </si>
+  <si>
+    <t>Public reserve</t>
+  </si>
+  <si>
+    <t>Special reserve</t>
+  </si>
+  <si>
+    <t>Fair value reserve</t>
+  </si>
+  <si>
+    <t>Reserve of cash flow hedges</t>
+  </si>
+  <si>
+    <t>Other reserves</t>
+  </si>
+  <si>
+    <t>Total equity attributable to owners of parent</t>
+  </si>
+  <si>
+    <t>15,510,605</t>
+  </si>
+  <si>
+    <t>7,040,359</t>
+  </si>
+  <si>
+    <t>Non-controlling interests</t>
+  </si>
+  <si>
+    <t>1,243,704</t>
+  </si>
+  <si>
+    <t>1,007,057</t>
+  </si>
+  <si>
+    <t>Total equity</t>
+  </si>
+  <si>
+    <t>16,754,309</t>
+  </si>
+  <si>
+    <t>8,047,416</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>Non-current liabilities</t>
+  </si>
+  <si>
+    <t>Non-current provisions</t>
+  </si>
+  <si>
+    <t>Non current borrowings</t>
+  </si>
+  <si>
+    <t>535,626</t>
+  </si>
+  <si>
+    <t>16,001,533</t>
+  </si>
+  <si>
+    <t>Trade and other non-current payables</t>
+  </si>
+  <si>
+    <t>Non-current payables to related parties</t>
+  </si>
+  <si>
+    <t>Deferred tax liabilities</t>
+  </si>
+  <si>
+    <t>Non-current finance lease obligations</t>
+  </si>
+  <si>
+    <t>670,811</t>
+  </si>
+  <si>
+    <t>725,731</t>
+  </si>
+  <si>
+    <t>Other non-current financial liabilities</t>
+  </si>
+  <si>
+    <t>Other non-current liabilities</t>
+  </si>
+  <si>
+    <t>Total non-current liabilities</t>
+  </si>
+  <si>
+    <t>1,206,437</t>
+  </si>
+  <si>
+    <t>16,727,264</t>
+  </si>
+  <si>
+    <t>Current liabilities</t>
+  </si>
+  <si>
+    <t>Current provisions</t>
+  </si>
+  <si>
+    <t>Current borrowings</t>
+  </si>
+  <si>
+    <t>155,592</t>
+  </si>
+  <si>
+    <t>3,207,336</t>
+  </si>
+  <si>
+    <t>Trade and other current payables</t>
+  </si>
+  <si>
+    <t>11,908,817</t>
+  </si>
+  <si>
+    <t>11,726,935</t>
+  </si>
+  <si>
+    <t>Current payables to related parties</t>
+  </si>
+  <si>
+    <t>10,000,000</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Bank overdraft</t>
+  </si>
+  <si>
+    <t>169,636</t>
+  </si>
+  <si>
+    <t>118,724</t>
+  </si>
+  <si>
+    <t>Current finance lease obligations</t>
+  </si>
+  <si>
+    <t>65,000</t>
+  </si>
+  <si>
+    <t>13,750</t>
+  </si>
+  <si>
+    <t>Other current financial liabilities</t>
+  </si>
+  <si>
+    <t>Income tax provision</t>
+  </si>
+  <si>
+    <t>Refundable deposits</t>
+  </si>
+  <si>
+    <t>Revenue received in advance, current</t>
+  </si>
+  <si>
+    <t>Other current liabilities</t>
+  </si>
+  <si>
+    <t>Total current liabilities</t>
+  </si>
+  <si>
+    <t>22,299,045</t>
+  </si>
+  <si>
+    <t>15,066,745</t>
+  </si>
+  <si>
+    <t>Total liabilities</t>
+  </si>
+  <si>
+    <t>23,505,482</t>
+  </si>
+  <si>
+    <t>31,794,009</t>
+  </si>
+  <si>
+    <t>Total equity and liabilities</t>
+  </si>
+  <si>
+    <t>Profit (loss)</t>
+  </si>
+  <si>
+    <t>Operating revenue</t>
+  </si>
+  <si>
+    <t>1,243,199</t>
+  </si>
+  <si>
+    <t>855,841</t>
+  </si>
+  <si>
+    <t>Operating expense</t>
+  </si>
+  <si>
+    <t>1,664,651</t>
+  </si>
+  <si>
+    <t>1,691,089</t>
+  </si>
+  <si>
+    <t>Gross profit</t>
+  </si>
+  <si>
+    <t>-421,452</t>
+  </si>
+  <si>
+    <t>-835,248</t>
+  </si>
+  <si>
+    <t>General and administrative expenses</t>
+  </si>
+  <si>
+    <t>331,624</t>
+  </si>
+  <si>
+    <t>284,329</t>
+  </si>
+  <si>
+    <t>Selling and distribution expenses</t>
+  </si>
+  <si>
+    <t>Government revenue share</t>
+  </si>
+  <si>
+    <t>Business support fees and brand fees</t>
+  </si>
+  <si>
+    <t>Other operating expense</t>
+  </si>
+  <si>
+    <t>Profit (loss) from operating activities</t>
+  </si>
+  <si>
+    <t>-753,076</t>
+  </si>
+  <si>
+    <t>-1,119,577</t>
+  </si>
+  <si>
+    <t>Other provisions</t>
+  </si>
+  <si>
+    <t>Other income</t>
+  </si>
+  <si>
+    <t>9,774,253</t>
+  </si>
+  <si>
+    <t>924,543</t>
+  </si>
+  <si>
+    <t>Other expense</t>
+  </si>
+  <si>
+    <t>Realized gains (losses) on financial assets at fair value through other comprehensive income</t>
+  </si>
+  <si>
+    <t>-553,395</t>
+  </si>
+  <si>
+    <t>Gains (losses) on financial assets at fair value through income statement</t>
+  </si>
+  <si>
+    <t>Finance income</t>
+  </si>
+  <si>
+    <t>Finance costs</t>
+  </si>
+  <si>
+    <t>190,397</t>
+  </si>
+  <si>
+    <t>290,495</t>
+  </si>
+  <si>
+    <t>Gains on investments in subsidiaries, joint ventures and associates</t>
+  </si>
+  <si>
+    <t>Profit (loss) before tax from continuous operations</t>
+  </si>
+  <si>
+    <t>8,830,780</t>
+  </si>
+  <si>
+    <t>-1,038,924</t>
+  </si>
+  <si>
+    <t>Income tax expense</t>
+  </si>
+  <si>
+    <t>123,887</t>
+  </si>
+  <si>
+    <t>45,087</t>
+  </si>
+  <si>
+    <t>Profit (loss) from continuing operations</t>
+  </si>
+  <si>
+    <t>8,706,893</t>
+  </si>
+  <si>
+    <t>-1,084,011</t>
+  </si>
+  <si>
+    <t>Profit (loss) from discontinued operations</t>
+  </si>
+  <si>
+    <t>Profit (loss), attributable to</t>
+  </si>
+  <si>
+    <t>Profit (loss), attributable to owners of parent</t>
+  </si>
+  <si>
+    <t>8,470,246</t>
+  </si>
+  <si>
+    <t>-1,169,013</t>
+  </si>
+  <si>
+    <t>Profit (loss), attributable to non-controlling interests</t>
+  </si>
+  <si>
+    <t>236,647</t>
+  </si>
+  <si>
+    <t>85,002</t>
+  </si>
+  <si>
+    <t>Earnings per share</t>
+  </si>
+  <si>
+    <t>Basic earnings (loss) per share</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>-0.08</t>
+  </si>
+  <si>
+    <t>Diluted earnings (loss) per share</t>
+  </si>
+  <si>
+    <t>Total investments in subsidiaries, joint ventures and associates</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Non-current trade receivables</t>
+  </si>
+  <si>
+    <t>Non-current receivables from sale of properties</t>
+  </si>
+  <si>
+    <t>Non-current receivables from rental of properties</t>
+  </si>
+  <si>
+    <t>Other non-current receivables</t>
+  </si>
+  <si>
+    <t>Total trade and other non-current receivables</t>
+  </si>
+  <si>
+    <t>Current materials and supplies to be consumed in production process or rendering services</t>
+  </si>
+  <si>
+    <t>Food and drinks</t>
+  </si>
+  <si>
+    <t>Current supplies &amp; stationeries</t>
+  </si>
+  <si>
+    <t>Medicines and medical supplies</t>
+  </si>
+  <si>
+    <t>Current oil and stations supplies</t>
+  </si>
+  <si>
+    <t>Medicine and pharmacy materials</t>
+  </si>
+  <si>
+    <t>Operation and clinics materials</t>
+  </si>
+  <si>
+    <t>Non-medical materials and stationary warehouse</t>
+  </si>
+  <si>
+    <t>Labs materials</t>
+  </si>
+  <si>
+    <t>Books and uniforms</t>
+  </si>
+  <si>
+    <t>Total current materials and supplies to be consumed in production process or rendering services</t>
+  </si>
+  <si>
+    <t>Current raw materials</t>
+  </si>
+  <si>
+    <t>Material and supplies</t>
+  </si>
+  <si>
+    <t>Current finished goods</t>
+  </si>
+  <si>
+    <t>Current spare parts</t>
+  </si>
+  <si>
+    <t>Current fuel</t>
+  </si>
+  <si>
+    <t>Current inventories in transit</t>
+  </si>
+  <si>
+    <t>Other current inventories</t>
+  </si>
+  <si>
+    <t>Current artificial grass</t>
+  </si>
+  <si>
+    <t>Current grass fixing and playground tools</t>
+  </si>
+  <si>
+    <t>Current playground floors and other equipments</t>
+  </si>
+  <si>
+    <t>Current strategic fuel inventory</t>
+  </si>
+  <si>
+    <t>Current grocery items</t>
+  </si>
+  <si>
+    <t>Current handsets and others</t>
+  </si>
+  <si>
+    <t>Total other current inventories</t>
+  </si>
+  <si>
+    <t>Provision for slow and damaged inventories</t>
+  </si>
+  <si>
+    <t>Provision for impairment of inventory</t>
+  </si>
+  <si>
+    <t>Total current inventories</t>
+  </si>
+  <si>
+    <t>Current trade receivables</t>
+  </si>
+  <si>
+    <t>Current receivables due from telecom operators</t>
+  </si>
+  <si>
+    <t>Current receivables from students</t>
+  </si>
+  <si>
+    <t>Notes receivable, current</t>
+  </si>
+  <si>
+    <t>Checks under collection, current</t>
+  </si>
+  <si>
+    <t>Current receivables from rental of properties</t>
+  </si>
+  <si>
+    <t>Legal cases receivables, current</t>
+  </si>
+  <si>
+    <t>Current receivables due from shareholders</t>
+  </si>
+  <si>
+    <t>Other current receivables</t>
+  </si>
+  <si>
+    <t>Trade and other current receivables, gross</t>
+  </si>
+  <si>
+    <t>Provision for doubtful trade and other current receivables</t>
+  </si>
+  <si>
+    <t>Total trade and other current receivables</t>
+  </si>
+  <si>
+    <t>Current prepaid expenses</t>
+  </si>
+  <si>
+    <t>Current accrued income</t>
+  </si>
+  <si>
+    <t>Current advances to suppliers</t>
+  </si>
+  <si>
+    <t>Income tax deposits, current</t>
+  </si>
+  <si>
+    <t>Sales tax deposits, current</t>
+  </si>
+  <si>
+    <t>Government deposits, current</t>
+  </si>
+  <si>
+    <t>Current refundable deposits</t>
+  </si>
+  <si>
+    <t>Guarantees and deposits, current</t>
+  </si>
+  <si>
+    <t>Letter of credit, current</t>
+  </si>
+  <si>
+    <t>Current restricted cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Current receivables from lessors for maintenance claims</t>
+  </si>
+  <si>
+    <t>Bank margins, current</t>
+  </si>
+  <si>
+    <t>Other current assets, others</t>
+  </si>
+  <si>
+    <t>Total other current assets</t>
   </si>
 </sst>
 </file>
@@ -364,34 +1072,790 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:FE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:161">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>139</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>140</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>141</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>142</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>143</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>146</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>147</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>150</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>154</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>155</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>162</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>165</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>168</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>169</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>170</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>176</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>177</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>180</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>181</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>182</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>183</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>184</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>185</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>186</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>187</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>188</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>189</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>190</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>191</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>192</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>193</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>194</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>195</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>198</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>200</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>202</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>203</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>204</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>205</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>206</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>207</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>208</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>209</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>210</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>211</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>212</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>213</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>214</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>215</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>216</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>217</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>218</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>219</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>220</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>221</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>222</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>223</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>224</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>225</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>226</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>227</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>228</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>229</v>
+      </c>
+      <c r="ET1" t="s">
+        <v>230</v>
+      </c>
+      <c r="EU1" t="s">
+        <v>231</v>
+      </c>
+      <c r="EV1" t="s">
+        <v>232</v>
+      </c>
+      <c r="EW1" t="s">
+        <v>233</v>
+      </c>
+      <c r="EX1" t="s">
+        <v>234</v>
+      </c>
+      <c r="EY1" t="s">
+        <v>235</v>
+      </c>
+      <c r="EZ1" t="s">
+        <v>236</v>
+      </c>
+      <c r="FA1" t="s">
+        <v>237</v>
+      </c>
+      <c r="FB1" t="s">
+        <v>238</v>
+      </c>
+      <c r="FC1" t="s">
+        <v>239</v>
+      </c>
+      <c r="FD1" t="s">
+        <v>240</v>
+      </c>
+      <c r="FE1" t="s">
+        <v>241</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:161">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>144</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>152</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>156</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>160</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>163</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>166</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>174</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>178</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>178</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>29</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:161">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>129</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>138</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>145</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>149</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>157</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>161</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>164</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>167</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>179</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>179</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>30</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>